<commit_message>
refactor to only pass references to Mat instead of using subviews
</commit_message>
<xml_diff>
--- a/datasets/careval.xlsx
+++ b/datasets/careval.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9704" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9712" uniqueCount="34">
   <si>
     <t>vhigh</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>doors x class</t>
+  </si>
+  <si>
+    <t>Neg sum</t>
+  </si>
+  <si>
+    <t>Cond entropy</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>InfoGain</t>
   </si>
 </sst>
 </file>
@@ -19268,7 +19280,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A23:F29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0"/>
@@ -19349,7 +19361,88 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="7"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of id" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:F18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0">
@@ -21157,89 +21250,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="5">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="7"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of id" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K12:P14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0"/>
@@ -21561,10 +21573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F29"/>
+  <dimension ref="A2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21577,12 +21589,12 @@
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -21590,7 +21602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -21609,8 +21621,26 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -21625,8 +21655,24 @@
       <c r="F5" s="3">
         <v>432</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <f>(GETPIVOTDATA("id",$A$3,"buying","high","class","acc")/GETPIVOTDATA("id",$A$3,"buying","high"))*LOG(GETPIVOTDATA("id",$A$3,"buying","high","class","acc")/GETPIVOTDATA("id",$A$3,"buying","high"), 2)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="J5">
+        <f>(GETPIVOTDATA("id",$A$3,"buying","high","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","high"))*LOG(GETPIVOTDATA("id",$A$3,"buying","high","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","high"), 2)</f>
+        <v>-0.31127812445913283</v>
+      </c>
+      <c r="L5">
+        <f>-SUM(H5:K5)</f>
+        <v>0.81127812445913283</v>
+      </c>
+      <c r="M5">
+        <f>L5*(GETPIVOTDATA("id",$A$3,"buying","high")/GETPIVOTDATA("id",$A$3))</f>
+        <v>0.20281953111478321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -21645,8 +21691,32 @@
       <c r="F6" s="3">
         <v>432</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <f>GETPIVOTDATA("id",$A$3,"buying","low","class","acc")/GETPIVOTDATA("id",$A$3,"buying","low")*LOG(GETPIVOTDATA("id",$A$3,"buying","low","class","acc")/GETPIVOTDATA("id",$A$3,"buying","low"),2)</f>
+        <v>-0.46954794522347054</v>
+      </c>
+      <c r="I6">
+        <f>GETPIVOTDATA("id",$A$3,"buying","low","class","good")/GETPIVOTDATA("id",$A$3,"buying","low")*LOG(GETPIVOTDATA("id",$A$3,"buying","low","class","good")/GETPIVOTDATA("id",$A$3,"buying","low"),2)</f>
+        <v>-0.34407633129837262</v>
+      </c>
+      <c r="J6">
+        <f>GETPIVOTDATA("id",$A$3,"buying","low","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","low")*LOG(GETPIVOTDATA("id",$A$3,"buying","low","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","low"),2)</f>
+        <v>-0.44413042513651696</v>
+      </c>
+      <c r="K6">
+        <f>GETPIVOTDATA("id",$A$3,"buying","low","class","vgood")/GETPIVOTDATA("id",$A$3,"buying","low")*LOG(GETPIVOTDATA("id",$A$3,"buying","low","class","vgood")/GETPIVOTDATA("id",$A$3,"buying","low"),2)</f>
+        <v>-0.31321742140913794</v>
+      </c>
+      <c r="L6">
+        <f>-SUM(H6:K6)</f>
+        <v>1.570972123067498</v>
+      </c>
+      <c r="M6">
+        <f>L6*GETPIVOTDATA("id",$A$3,"buying","low")/GETPIVOTDATA("id",$A$3)</f>
+        <v>0.39274303076687445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -21665,8 +21735,32 @@
       <c r="F7" s="3">
         <v>432</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <f>GETPIVOTDATA("id",$A$3,"buying","med","class","acc")/GETPIVOTDATA("id",$A$3,"buying","med")*LOG(GETPIVOTDATA("id",$A$3,"buying","med","class","acc")/GETPIVOTDATA("id",$A$3,"buying","med"),2)</f>
+        <v>-0.50828867335693462</v>
+      </c>
+      <c r="I7">
+        <f>GETPIVOTDATA("id",$A$3,"buying","med","class","good")/GETPIVOTDATA("id",$A$3,"buying","med")*LOG(GETPIVOTDATA("id",$A$3,"buying","med","class","good")/GETPIVOTDATA("id",$A$3,"buying","med"),2)</f>
+        <v>-0.22527890638992706</v>
+      </c>
+      <c r="J7">
+        <f>GETPIVOTDATA("id",$A$3,"buying","med","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","med")*LOG(GETPIVOTDATA("id",$A$3,"buying","med","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","med"),2)</f>
+        <v>-0.42731006374334851</v>
+      </c>
+      <c r="K7">
+        <f>GETPIVOTDATA("id",$A$3,"buying","med","class","vgood")/GETPIVOTDATA("id",$A$3,"buying","med")*LOG(GETPIVOTDATA("id",$A$3,"buying","med","class","vgood")/GETPIVOTDATA("id",$A$3,"buying","med"),2)</f>
+        <v>-0.24401769070505042</v>
+      </c>
+      <c r="L7">
+        <f>-SUM(H7:K7)</f>
+        <v>1.4048953341952606</v>
+      </c>
+      <c r="M7">
+        <f>L7*GETPIVOTDATA("id",$A$3,"buying","med")/GETPIVOTDATA("id",$A$3)</f>
+        <v>0.35122383354881515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -21681,8 +21775,24 @@
       <c r="F8" s="3">
         <v>432</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <f>GETPIVOTDATA("id",$A$3,"buying","vhigh","class","acc")/GETPIVOTDATA("id",$A$3,"buying","vhigh")*LOG(GETPIVOTDATA("id",$A$3,"buying","vhigh","class","acc")/GETPIVOTDATA("id",$A$3,"buying","vhigh"),2)</f>
+        <v>-0.43082708345352599</v>
+      </c>
+      <c r="J8">
+        <f>GETPIVOTDATA("id",$A$3,"buying","vhigh","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","vhigh")*LOG(GETPIVOTDATA("id",$A$3,"buying","vhigh","class","unacc")/GETPIVOTDATA("id",$A$3,"buying","vhigh"),2)</f>
+        <v>-0.21919533819482817</v>
+      </c>
+      <c r="L8">
+        <f>-SUM(H8:K8)</f>
+        <v>0.65002242164835411</v>
+      </c>
+      <c r="M8">
+        <f>L8*GETPIVOTDATA("id",$A$3,"buying","vhigh")/GETPIVOTDATA("id",$A$3)</f>
+        <v>0.16250560541208856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -21702,12 +21812,30 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10">
+        <f>SUM(M5:M8)</f>
+        <v>1.1092920008425613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11">
+        <f>data!L18-'contingency tables'!M10</f>
+        <v>9.6448969169613763E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -21715,7 +21843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -21735,7 +21863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -21755,7 +21883,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -21950,16 +22078,16 @@
   <dimension ref="A1:P1729"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>

</xml_diff>